<commit_message>
consolidated 13 nov characterization flows
</commit_message>
<xml_diff>
--- a/data/1311021 cv-char4.xlsx
+++ b/data/1311021 cv-char4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6383,16 +6383,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>140493</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>121443</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>102393</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>347663</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6703,7 +6703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -9718,8 +9718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F453"/>
   <sheetViews>
-    <sheetView topLeftCell="A424" workbookViewId="0">
-      <selection activeCell="A304" sqref="A304:F453"/>
+    <sheetView tabSelected="1" topLeftCell="A433" workbookViewId="0">
+      <selection activeCell="E453" sqref="E453"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>